<commit_message>
Revert "Merge branch 'staging' into bot-tools"
This reverts commit 65006ba6655224065d5ed52f7c6043757d7dff64, reversing
changes made to 2726308bbb13dc534b6c58860863efa9ec2b74d0.
</commit_message>
<xml_diff>
--- a/add-matchs-tool/data/round_table_matchs1.xlsx
+++ b/add-matchs-tool/data/round_table_matchs1.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenkhoa/Desktop/firebird/testnet-minigame/add-matchs-tool/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5161221-5F9A-6C40-B840-50C8090D5B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFCA0E3-8F70-C347-8B01-B60217F68CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1100" windowWidth="38400" windowHeight="20080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1100" windowWidth="38400" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId2"/>
-    <sheet name="Round table" sheetId="1" r:id="rId3"/>
-    <sheet name="Sumary" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="test" sheetId="4" r:id="rId1"/>
+    <sheet name="Round table" sheetId="1" r:id="rId2"/>
+    <sheet name="Sumary" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Round table'!#REF!</definedName>
-    <definedName name="Z_BE3B438B_38A7_4CD8_8BE7_9E446A9B2CDC_.wvu.FilterData" localSheetId="2" hidden="1">'Round table'!#REF!</definedName>
-    <definedName name="Z_EE2F20B3_2CAB_4FD8_97BE_93C792EE71D7_.wvu.FilterData" localSheetId="2" hidden="1">'Round table'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Round table'!#REF!</definedName>
+    <definedName name="Z_BE3B438B_38A7_4CD8_8BE7_9E446A9B2CDC_.wvu.FilterData" localSheetId="1" hidden="1">'Round table'!#REF!</definedName>
+    <definedName name="Z_EE2F20B3_2CAB_4FD8_97BE_93C792EE71D7_.wvu.FilterData" localSheetId="1" hidden="1">'Round table'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="149">
   <si>
     <t>Type</t>
   </si>
@@ -468,19 +467,28 @@
     <t>SERBIA</t>
   </si>
   <si>
-    <t>Trang admin</t>
+    <t>NEW ZEALAND</t>
   </si>
   <si>
-    <t>Api log FE error</t>
+    <t>HENAN</t>
   </si>
   <si>
-    <t>Xem history của người chơi khác</t>
+    <t>SHANDONG</t>
   </si>
   <si>
-    <t>Leaderborad history responsive</t>
+    <t>SHAANXI CHANG</t>
   </si>
   <si>
-    <t>Fix bug invaid nonce</t>
+    <t>JIANGSU</t>
+  </si>
+  <si>
+    <t>WUHAN</t>
+  </si>
+  <si>
+    <t>SHANGHAI</t>
+  </si>
+  <si>
+    <t>THAILAND</t>
   </si>
 </sst>
 </file>
@@ -809,6 +817,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,7 +851,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,14 +1065,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9902AC12-1A76-1B44-AEED-7468B00A6025}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7397E85-945B-0546-BEFA-D5BE54DFF40F}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:27" s="30" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
@@ -1149,45 +1166,45 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47">
-        <v>101</v>
-      </c>
-      <c r="B2" s="47">
-        <v>1668960000</v>
-      </c>
-      <c r="C2" s="47">
-        <v>10230541</v>
+    <row r="2" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="48">
+        <v>35</v>
+      </c>
+      <c r="B2" s="48">
+        <v>1668488400</v>
+      </c>
+      <c r="C2" s="48">
+        <v>10859947</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="47">
-        <v>7643</v>
-      </c>
-      <c r="F2" s="47">
-        <v>0</v>
-      </c>
-      <c r="G2" s="47">
+        <v>141</v>
+      </c>
+      <c r="E2" s="48">
+        <v>56746</v>
+      </c>
+      <c r="F2" s="48">
+        <v>0</v>
+      </c>
+      <c r="G2" s="48">
         <v>0</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" s="47">
-        <v>21</v>
-      </c>
-      <c r="J2" s="47">
-        <v>0</v>
-      </c>
-      <c r="K2" s="47">
+        <v>136</v>
+      </c>
+      <c r="I2" s="48">
+        <v>11</v>
+      </c>
+      <c r="J2" s="48">
+        <v>0</v>
+      </c>
+      <c r="K2" s="48">
         <v>0</v>
       </c>
       <c r="L2" s="32" t="s">
         <v>103</v>
       </c>
       <c r="M2" s="32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N2" s="32">
         <v>0</v>
@@ -1232,60 +1249,60 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="47">
-        <v>102</v>
-      </c>
-      <c r="B3" s="47">
-        <v>1669035600</v>
-      </c>
-      <c r="C3" s="47">
-        <v>10230543</v>
+    <row r="3" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="48">
+        <v>36</v>
+      </c>
+      <c r="B3" s="48">
+        <v>1668492000</v>
+      </c>
+      <c r="C3" s="48">
+        <v>10853471</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="47">
-        <v>16</v>
-      </c>
-      <c r="F3" s="47">
-        <v>0</v>
-      </c>
-      <c r="G3" s="47">
+        <v>142</v>
+      </c>
+      <c r="E3" s="48">
+        <v>39121</v>
+      </c>
+      <c r="F3" s="48">
+        <v>0</v>
+      </c>
+      <c r="G3" s="48">
         <v>0</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="I3" s="47">
-        <v>28</v>
-      </c>
-      <c r="J3" s="47">
-        <v>0</v>
-      </c>
-      <c r="K3" s="47">
+        <v>143</v>
+      </c>
+      <c r="I3" s="48">
+        <v>80691</v>
+      </c>
+      <c r="J3" s="48">
+        <v>0</v>
+      </c>
+      <c r="K3" s="48">
         <v>0</v>
       </c>
       <c r="L3" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="32">
+        <v>3</v>
+      </c>
+      <c r="N3" s="32">
+        <v>0</v>
+      </c>
+      <c r="O3" s="32">
+        <v>0</v>
+      </c>
+      <c r="P3" s="32">
+        <v>2.12</v>
+      </c>
+      <c r="Q3" s="48">
         <v>1</v>
       </c>
-      <c r="N3" s="32">
-        <v>0</v>
-      </c>
-      <c r="O3" s="32">
-        <v>0</v>
-      </c>
-      <c r="P3" s="32">
-        <v>1.56</v>
-      </c>
-      <c r="Q3" s="47">
-        <v>0.5</v>
-      </c>
       <c r="R3" s="32">
-        <v>2.7</v>
+        <v>1.86</v>
       </c>
       <c r="S3" s="32">
         <v>2.09</v>
@@ -1302,73 +1319,73 @@
       <c r="W3" s="32">
         <v>2.4</v>
       </c>
-      <c r="X3" s="47">
+      <c r="X3" s="48">
         <v>11</v>
       </c>
       <c r="Y3" s="32">
-        <v>1.33</v>
+        <v>2.33</v>
       </c>
       <c r="Z3" s="32">
+        <v>2.25</v>
+      </c>
+      <c r="AA3" s="48">
         <v>5.25</v>
       </c>
-      <c r="AA3" s="47">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="47">
-        <v>103</v>
-      </c>
-      <c r="B4" s="47">
-        <v>1669046400</v>
-      </c>
-      <c r="C4" s="47">
-        <v>10230533</v>
+    </row>
+    <row r="4" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="48">
+        <v>37</v>
+      </c>
+      <c r="B4" s="48">
+        <v>1668492000</v>
+      </c>
+      <c r="C4" s="48">
+        <v>10853472</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="47">
-        <v>1043</v>
-      </c>
-      <c r="F4" s="47">
-        <v>0</v>
-      </c>
-      <c r="G4" s="47">
+        <v>144</v>
+      </c>
+      <c r="E4" s="48">
+        <v>5448</v>
+      </c>
+      <c r="F4" s="48">
+        <v>0</v>
+      </c>
+      <c r="G4" s="48">
         <v>0</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="47">
-        <v>36</v>
-      </c>
-      <c r="J4" s="47">
-        <v>0</v>
-      </c>
-      <c r="K4" s="47">
+        <v>145</v>
+      </c>
+      <c r="I4" s="48">
+        <v>20772</v>
+      </c>
+      <c r="J4" s="48">
+        <v>0</v>
+      </c>
+      <c r="K4" s="48">
         <v>0</v>
       </c>
       <c r="L4" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="32">
+        <v>3</v>
+      </c>
+      <c r="N4" s="32">
+        <v>0</v>
+      </c>
+      <c r="O4" s="32">
+        <v>0</v>
+      </c>
+      <c r="P4" s="32">
+        <v>2.06</v>
+      </c>
+      <c r="Q4" s="48">
         <v>1</v>
       </c>
-      <c r="N4" s="32">
-        <v>0</v>
-      </c>
-      <c r="O4" s="32">
-        <v>0</v>
-      </c>
-      <c r="P4" s="32">
-        <v>1.5</v>
-      </c>
-      <c r="Q4" s="47">
-        <v>0.5</v>
-      </c>
       <c r="R4" s="32">
-        <v>2.75</v>
+        <v>1.85</v>
       </c>
       <c r="S4" s="32">
         <v>1.85</v>
@@ -1380,87 +1397,87 @@
         <v>2.09</v>
       </c>
       <c r="V4" s="32">
-        <v>6.03</v>
+        <v>4.03</v>
       </c>
       <c r="W4" s="32">
         <v>2.25</v>
       </c>
       <c r="X4" s="32">
-        <v>2.3199999999999998</v>
+        <v>3.32</v>
       </c>
       <c r="Y4" s="32">
-        <v>6.2</v>
+        <v>5.2</v>
       </c>
       <c r="Z4" s="32">
         <v>3.92</v>
       </c>
       <c r="AA4" s="32">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="47">
-        <v>104</v>
-      </c>
-      <c r="B5" s="47">
-        <v>1669057200</v>
-      </c>
-      <c r="C5" s="47">
-        <v>10230548</v>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="48">
+        <v>38</v>
+      </c>
+      <c r="B5" s="48">
+        <v>1668499200</v>
+      </c>
+      <c r="C5" s="48">
+        <v>10853518</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="47">
-        <v>37</v>
-      </c>
-      <c r="F5" s="47">
-        <v>0</v>
-      </c>
-      <c r="G5" s="47">
+        <v>146</v>
+      </c>
+      <c r="E5" s="48">
+        <v>5448</v>
+      </c>
+      <c r="F5" s="48">
+        <v>0</v>
+      </c>
+      <c r="G5" s="48">
         <v>0</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" s="47">
-        <v>7350</v>
-      </c>
-      <c r="J5" s="47">
-        <v>0</v>
-      </c>
-      <c r="K5" s="47">
+        <v>147</v>
+      </c>
+      <c r="I5" s="48">
+        <v>20772</v>
+      </c>
+      <c r="J5" s="48">
+        <v>0</v>
+      </c>
+      <c r="K5" s="48">
         <v>0</v>
       </c>
       <c r="L5" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="32">
+        <v>3</v>
+      </c>
+      <c r="N5" s="32">
+        <v>0</v>
+      </c>
+      <c r="O5" s="32">
+        <v>0</v>
+      </c>
+      <c r="P5" s="32">
+        <v>1.88</v>
+      </c>
+      <c r="Q5" s="48">
         <v>1</v>
       </c>
-      <c r="N5" s="32">
-        <v>0</v>
-      </c>
-      <c r="O5" s="32">
-        <v>0</v>
-      </c>
-      <c r="P5" s="32">
-        <v>1.6</v>
-      </c>
-      <c r="Q5" s="47">
-        <v>0.5</v>
-      </c>
       <c r="R5" s="32">
-        <v>2.4500000000000002</v>
+        <v>2.11</v>
       </c>
       <c r="S5" s="32">
-        <v>1.55</v>
-      </c>
-      <c r="T5" s="47">
-        <v>1.5</v>
+        <v>1.9</v>
+      </c>
+      <c r="T5" s="48">
+        <v>2</v>
       </c>
       <c r="U5" s="32">
-        <v>2.7</v>
+        <v>2.1</v>
       </c>
       <c r="V5" s="32">
         <v>3.32</v>
@@ -1468,7 +1485,7 @@
       <c r="W5" s="32">
         <v>2.06</v>
       </c>
-      <c r="X5" s="47">
+      <c r="X5" s="48">
         <v>4</v>
       </c>
       <c r="Y5" s="32">
@@ -1481,87 +1498,87 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="47">
-        <v>105</v>
-      </c>
-      <c r="B6" s="47">
-        <v>1669111200</v>
-      </c>
-      <c r="C6" s="47">
-        <v>10230528</v>
+    <row r="6" spans="1:27" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="31">
+        <v>39</v>
+      </c>
+      <c r="B6" s="31">
+        <v>1668501000</v>
+      </c>
+      <c r="C6" s="31">
+        <v>10728739</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" s="47">
-        <v>24</v>
-      </c>
-      <c r="F6" s="47">
-        <v>0</v>
-      </c>
-      <c r="G6" s="47">
+        <v>123</v>
+      </c>
+      <c r="E6" s="32">
+        <v>11</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0</v>
+      </c>
+      <c r="G6" s="31">
         <v>0</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="47">
+        <v>148</v>
+      </c>
+      <c r="I6" s="31">
         <v>1489</v>
       </c>
-      <c r="J6" s="47">
-        <v>0</v>
-      </c>
-      <c r="K6" s="47">
+      <c r="J6" s="31">
+        <v>0</v>
+      </c>
+      <c r="K6" s="31">
         <v>0</v>
       </c>
       <c r="L6" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="M6" s="47">
+        <v>118</v>
+      </c>
+      <c r="M6" s="32">
+        <v>3</v>
+      </c>
+      <c r="N6" s="32">
+        <v>0</v>
+      </c>
+      <c r="O6" s="32">
+        <v>0</v>
+      </c>
+      <c r="P6" s="31">
+        <v>2.09</v>
+      </c>
+      <c r="Q6" s="32">
         <v>1</v>
       </c>
-      <c r="N6" s="32">
-        <v>0</v>
-      </c>
-      <c r="O6" s="32">
-        <v>0</v>
-      </c>
-      <c r="P6" s="32">
-        <v>2.59</v>
-      </c>
-      <c r="Q6" s="32">
-        <v>1.5</v>
-      </c>
       <c r="R6" s="32">
-        <v>1.56</v>
+        <v>1.85</v>
       </c>
       <c r="S6" s="32">
-        <v>1.69</v>
-      </c>
-      <c r="T6" s="47">
+        <v>2.09</v>
+      </c>
+      <c r="T6" s="31">
         <v>2.5</v>
       </c>
-      <c r="U6" s="47">
-        <v>2.35</v>
-      </c>
-      <c r="V6" s="32">
-        <v>1.65</v>
+      <c r="U6" s="31">
+        <v>1.88</v>
+      </c>
+      <c r="V6" s="31">
+        <v>2.3199999999999998</v>
       </c>
       <c r="W6" s="32">
-        <v>2.87</v>
+        <v>2.27</v>
       </c>
       <c r="X6" s="32">
-        <v>13.12</v>
+        <v>5.85</v>
       </c>
       <c r="Y6" s="32">
-        <v>1.2</v>
+        <v>1.68</v>
       </c>
       <c r="Z6" s="32">
-        <v>8.1</v>
-      </c>
-      <c r="AA6" s="47">
-        <v>23</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AA6" s="31">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>
@@ -1570,49 +1587,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEC6845-7DF7-BD41-A648-C34CD983C22E}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="87.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" s="48" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" s="48" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="48" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="48" t="s">
-        <v>145</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1620,8 +1594,8 @@
   </sheetPr>
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1717,38 +1691,38 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47">
+    <row r="2" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="48">
         <v>1</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="48">
         <v>1668960000</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="48">
         <v>10230541</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="47">
+      <c r="E2" s="48">
         <v>7643</v>
       </c>
-      <c r="F2" s="47">
-        <v>0</v>
-      </c>
-      <c r="G2" s="47">
+      <c r="F2" s="48">
+        <v>0</v>
+      </c>
+      <c r="G2" s="48">
         <v>0</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="47">
+      <c r="I2" s="48">
         <v>21</v>
       </c>
-      <c r="J2" s="47">
-        <v>0</v>
-      </c>
-      <c r="K2" s="47">
+      <c r="J2" s="48">
+        <v>0</v>
+      </c>
+      <c r="K2" s="48">
         <v>0</v>
       </c>
       <c r="L2" s="32" t="s">
@@ -1800,44 +1774,44 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="47">
+    <row r="3" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="48">
         <v>1669035600</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="48">
         <v>10230543</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="48">
         <v>16</v>
       </c>
-      <c r="F3" s="47">
-        <v>0</v>
-      </c>
-      <c r="G3" s="47">
+      <c r="F3" s="48">
+        <v>0</v>
+      </c>
+      <c r="G3" s="48">
         <v>0</v>
       </c>
       <c r="H3" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="48">
         <v>28</v>
       </c>
-      <c r="J3" s="47">
-        <v>0</v>
-      </c>
-      <c r="K3" s="47">
+      <c r="J3" s="48">
+        <v>0</v>
+      </c>
+      <c r="K3" s="48">
         <v>0</v>
       </c>
       <c r="L3" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="48">
         <v>1</v>
       </c>
       <c r="N3" s="32">
@@ -1847,13 +1821,13 @@
         <v>0</v>
       </c>
       <c r="P3" s="32">
-        <v>1.56</v>
-      </c>
-      <c r="Q3" s="47">
-        <v>0.5</v>
+        <v>2.12</v>
+      </c>
+      <c r="Q3" s="48">
+        <v>1</v>
       </c>
       <c r="R3" s="32">
-        <v>2.7</v>
+        <v>1.86</v>
       </c>
       <c r="S3" s="32">
         <v>2.09</v>
@@ -1870,7 +1844,7 @@
       <c r="W3" s="32">
         <v>2.4</v>
       </c>
-      <c r="X3" s="47">
+      <c r="X3" s="48">
         <v>11</v>
       </c>
       <c r="Y3" s="32">
@@ -1879,48 +1853,48 @@
       <c r="Z3" s="32">
         <v>5.25</v>
       </c>
-      <c r="AA3" s="47">
+      <c r="AA3" s="48">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="47">
+    <row r="4" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="48">
         <v>3</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="48">
         <v>1669046400</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="48">
         <v>10230533</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="48">
         <v>1043</v>
       </c>
-      <c r="F4" s="47">
-        <v>0</v>
-      </c>
-      <c r="G4" s="47">
+      <c r="F4" s="48">
+        <v>0</v>
+      </c>
+      <c r="G4" s="48">
         <v>0</v>
       </c>
       <c r="H4" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="47">
+      <c r="I4" s="48">
         <v>36</v>
       </c>
-      <c r="J4" s="47">
-        <v>0</v>
-      </c>
-      <c r="K4" s="47">
+      <c r="J4" s="48">
+        <v>0</v>
+      </c>
+      <c r="K4" s="48">
         <v>0</v>
       </c>
       <c r="L4" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="47">
+      <c r="M4" s="48">
         <v>1</v>
       </c>
       <c r="N4" s="32">
@@ -1930,13 +1904,13 @@
         <v>0</v>
       </c>
       <c r="P4" s="32">
-        <v>1.5</v>
-      </c>
-      <c r="Q4" s="47">
-        <v>0.5</v>
+        <v>2.06</v>
+      </c>
+      <c r="Q4" s="48">
+        <v>1</v>
       </c>
       <c r="R4" s="32">
-        <v>2.75</v>
+        <v>1.85</v>
       </c>
       <c r="S4" s="32">
         <v>1.85</v>
@@ -1966,44 +1940,44 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="47">
+    <row r="5" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="48">
         <v>4</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="48">
         <v>1669057200</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="48">
         <v>10230548</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="48">
         <v>37</v>
       </c>
-      <c r="F5" s="47">
-        <v>0</v>
-      </c>
-      <c r="G5" s="47">
+      <c r="F5" s="48">
+        <v>0</v>
+      </c>
+      <c r="G5" s="48">
         <v>0</v>
       </c>
       <c r="H5" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="48">
         <v>7350</v>
       </c>
-      <c r="J5" s="47">
-        <v>0</v>
-      </c>
-      <c r="K5" s="47">
+      <c r="J5" s="48">
+        <v>0</v>
+      </c>
+      <c r="K5" s="48">
         <v>0</v>
       </c>
       <c r="L5" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="48">
         <v>1</v>
       </c>
       <c r="N5" s="32">
@@ -2013,22 +1987,22 @@
         <v>0</v>
       </c>
       <c r="P5" s="32">
-        <v>1.6</v>
-      </c>
-      <c r="Q5" s="47">
-        <v>0.5</v>
+        <v>1.88</v>
+      </c>
+      <c r="Q5" s="48">
+        <v>1</v>
       </c>
       <c r="R5" s="32">
-        <v>2.4500000000000002</v>
+        <v>2.11</v>
       </c>
       <c r="S5" s="32">
-        <v>1.55</v>
-      </c>
-      <c r="T5" s="47">
-        <v>1.5</v>
+        <v>1.9</v>
+      </c>
+      <c r="T5" s="48">
+        <v>2</v>
       </c>
       <c r="U5" s="32">
-        <v>2.7</v>
+        <v>2.1</v>
       </c>
       <c r="V5" s="32">
         <v>3.32</v>
@@ -2036,7 +2010,7 @@
       <c r="W5" s="32">
         <v>2.06</v>
       </c>
-      <c r="X5" s="47">
+      <c r="X5" s="48">
         <v>4</v>
       </c>
       <c r="Y5" s="32">
@@ -2049,44 +2023,44 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="47">
+    <row r="6" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="48">
         <v>1669111200</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="48">
         <v>10230528</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="48">
         <v>24</v>
       </c>
-      <c r="F6" s="47">
-        <v>0</v>
-      </c>
-      <c r="G6" s="47">
+      <c r="F6" s="48">
+        <v>0</v>
+      </c>
+      <c r="G6" s="48">
         <v>0</v>
       </c>
       <c r="H6" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="48">
         <v>1489</v>
       </c>
-      <c r="J6" s="47">
-        <v>0</v>
-      </c>
-      <c r="K6" s="47">
+      <c r="J6" s="48">
+        <v>0</v>
+      </c>
+      <c r="K6" s="48">
         <v>0</v>
       </c>
       <c r="L6" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="47">
+      <c r="M6" s="48">
         <v>1</v>
       </c>
       <c r="N6" s="32">
@@ -2096,22 +2070,22 @@
         <v>0</v>
       </c>
       <c r="P6" s="32">
-        <v>2.59</v>
+        <v>2.21</v>
       </c>
       <c r="Q6" s="32">
         <v>1.5</v>
       </c>
       <c r="R6" s="32">
-        <v>1.56</v>
+        <v>1.75</v>
       </c>
       <c r="S6" s="32">
-        <v>1.69</v>
-      </c>
-      <c r="T6" s="47">
-        <v>2.5</v>
-      </c>
-      <c r="U6" s="47">
-        <v>2.35</v>
+        <v>1.94</v>
+      </c>
+      <c r="T6" s="48">
+        <v>3</v>
+      </c>
+      <c r="U6" s="48">
+        <v>2</v>
       </c>
       <c r="V6" s="32">
         <v>1.65</v>
@@ -2128,48 +2102,48 @@
       <c r="Z6" s="32">
         <v>8.1</v>
       </c>
-      <c r="AA6" s="47">
+      <c r="AA6" s="48">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="47">
+    <row r="7" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="48">
         <v>6</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="48">
         <v>1669122000</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="48">
         <v>10230576</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="48">
         <v>50</v>
       </c>
-      <c r="F7" s="47">
-        <v>0</v>
-      </c>
-      <c r="G7" s="47">
+      <c r="F7" s="48">
+        <v>0</v>
+      </c>
+      <c r="G7" s="48">
         <v>0</v>
       </c>
       <c r="H7" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="48">
         <v>56</v>
       </c>
-      <c r="J7" s="47">
-        <v>0</v>
-      </c>
-      <c r="K7" s="47">
+      <c r="J7" s="48">
+        <v>0</v>
+      </c>
+      <c r="K7" s="48">
         <v>0</v>
       </c>
       <c r="L7" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="48">
         <v>1</v>
       </c>
       <c r="N7" s="32">
@@ -2179,22 +2153,22 @@
         <v>0</v>
       </c>
       <c r="P7" s="32">
-        <v>1.48</v>
-      </c>
-      <c r="Q7" s="47">
-        <v>0.5</v>
+        <v>2.14</v>
+      </c>
+      <c r="Q7" s="32">
+        <v>1</v>
       </c>
       <c r="R7" s="32">
-        <v>2.8</v>
+        <v>1.83</v>
       </c>
       <c r="S7" s="32">
-        <v>2.2000000000000002</v>
+        <v>1.9</v>
       </c>
       <c r="T7" s="32">
         <v>2.5</v>
       </c>
-      <c r="U7" s="47">
-        <v>2.78</v>
+      <c r="U7" s="48">
+        <v>2.1</v>
       </c>
       <c r="V7" s="32">
         <v>2.2000000000000002</v>
@@ -2211,48 +2185,48 @@
       <c r="Z7" s="32">
         <v>4.7</v>
       </c>
-      <c r="AA7" s="47">
+      <c r="AA7" s="48">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="47">
+    <row r="8" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="48">
         <v>7</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="48">
         <v>1669132800</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="48">
         <v>10230565</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E8" s="48">
         <v>6</v>
       </c>
-      <c r="F8" s="47">
-        <v>0</v>
-      </c>
-      <c r="G8" s="47">
+      <c r="F8" s="48">
+        <v>0</v>
+      </c>
+      <c r="G8" s="48">
         <v>0</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="48">
         <v>7463</v>
       </c>
-      <c r="J8" s="47">
-        <v>0</v>
-      </c>
-      <c r="K8" s="47">
+      <c r="J8" s="48">
+        <v>0</v>
+      </c>
+      <c r="K8" s="48">
         <v>0</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="48">
         <v>1</v>
       </c>
       <c r="N8" s="32">
@@ -2264,20 +2238,20 @@
       <c r="P8" s="32">
         <v>1.78</v>
       </c>
-      <c r="Q8" s="47">
-        <v>0.5</v>
+      <c r="Q8" s="32">
+        <v>1</v>
       </c>
       <c r="R8" s="32">
-        <v>2.5299999999999998</v>
+        <v>2.16</v>
       </c>
       <c r="S8" s="32">
-        <v>2.5</v>
+        <v>1.06</v>
       </c>
       <c r="T8" s="32">
         <v>2.5</v>
       </c>
-      <c r="U8" s="47">
-        <v>1.6</v>
+      <c r="U8" s="48">
+        <v>1.87</v>
       </c>
       <c r="V8" s="32">
         <v>3.64</v>
@@ -2298,44 +2272,44 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="47">
+    <row r="9" spans="1:27" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="48">
         <v>8</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="48">
         <v>1669143600</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="48">
         <v>10230563</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="48">
         <v>22</v>
       </c>
-      <c r="F9" s="47">
-        <v>0</v>
-      </c>
-      <c r="G9" s="47">
+      <c r="F9" s="48">
+        <v>0</v>
+      </c>
+      <c r="G9" s="48">
         <v>0</v>
       </c>
       <c r="H9" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="47">
+      <c r="I9" s="48">
         <v>11</v>
       </c>
-      <c r="J9" s="47">
-        <v>0</v>
-      </c>
-      <c r="K9" s="47">
+      <c r="J9" s="48">
+        <v>0</v>
+      </c>
+      <c r="K9" s="48">
         <v>0</v>
       </c>
       <c r="L9" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="M9" s="47">
+      <c r="M9" s="48">
         <v>1</v>
       </c>
       <c r="N9" s="32">
@@ -2354,13 +2328,13 @@
         <v>1.85</v>
       </c>
       <c r="S9" s="32">
-        <v>1.73</v>
-      </c>
-      <c r="T9" s="32">
-        <v>2.5</v>
-      </c>
-      <c r="U9" s="47">
-        <v>2.33</v>
+        <v>1.88</v>
+      </c>
+      <c r="T9" s="48">
+        <v>3</v>
+      </c>
+      <c r="U9" s="48">
+        <v>2.04</v>
       </c>
       <c r="V9" s="32">
         <v>1.72</v>
@@ -2377,7 +2351,7 @@
       <c r="Z9" s="32">
         <v>6.7</v>
       </c>
-      <c r="AA9" s="47">
+      <c r="AA9" s="48">
         <v>14</v>
       </c>
     </row>
@@ -2409,10 +2383,10 @@
       <c r="I10" s="31">
         <v>5</v>
       </c>
-      <c r="J10" s="47">
-        <v>0</v>
-      </c>
-      <c r="K10" s="47">
+      <c r="J10" s="48">
+        <v>0</v>
+      </c>
+      <c r="K10" s="48">
         <v>0</v>
       </c>
       <c r="L10" s="32" t="s">
@@ -2511,22 +2485,22 @@
         <v>0</v>
       </c>
       <c r="P11" s="32">
-        <v>2.76</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q11" s="32">
         <v>1.5</v>
       </c>
       <c r="R11" s="32">
-        <v>1.54</v>
+        <v>1.79</v>
       </c>
       <c r="S11" s="32">
-        <v>1.74</v>
+        <v>1.92</v>
       </c>
       <c r="T11" s="31">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U11" s="31">
-        <v>2.25</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="V11" s="32">
         <v>2.04</v>
@@ -2594,22 +2568,22 @@
         <v>0</v>
       </c>
       <c r="P12" s="32">
-        <v>2.2000000000000002</v>
+        <v>1.81</v>
       </c>
       <c r="Q12" s="32">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R12" s="32">
-        <v>1.76</v>
+        <v>2.14</v>
       </c>
       <c r="S12" s="32">
-        <v>2.85</v>
+        <v>2.11</v>
       </c>
       <c r="T12" s="31">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U12" s="31">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="V12" s="32">
         <v>1.7</v>
@@ -2677,22 +2651,22 @@
         <v>0</v>
       </c>
       <c r="P13" s="32">
-        <v>2.79</v>
+        <v>1.8</v>
       </c>
       <c r="Q13" s="32">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R13" s="32">
-        <v>1.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="S13" s="32">
-        <v>1.82</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="T13" s="31">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U13" s="31">
-        <v>2.13</v>
+        <v>1.97</v>
       </c>
       <c r="V13" s="32">
         <v>1.96</v>
@@ -2760,22 +2734,22 @@
         <v>0</v>
       </c>
       <c r="P14" s="32">
-        <v>1.55</v>
-      </c>
-      <c r="Q14" s="31">
-        <v>0.5</v>
+        <v>1.9</v>
+      </c>
+      <c r="Q14" s="32">
+        <v>1</v>
       </c>
       <c r="R14" s="32">
-        <v>2.6</v>
+        <v>2.06</v>
       </c>
       <c r="S14" s="32">
-        <v>1.46</v>
+        <v>1.91</v>
       </c>
       <c r="T14" s="31">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="U14" s="31">
-        <v>2.98</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="V14" s="32">
         <v>2.61</v>
@@ -2845,8 +2819,8 @@
       <c r="P15" s="32">
         <v>1.83</v>
       </c>
-      <c r="Q15" s="31">
-        <v>0.5</v>
+      <c r="Q15" s="32">
+        <v>1</v>
       </c>
       <c r="R15" s="32">
         <v>2.12</v>
@@ -2926,22 +2900,22 @@
         <v>0</v>
       </c>
       <c r="P16" s="32">
-        <v>3.29</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Q16" s="32">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R16" s="32">
-        <v>1.4</v>
+        <v>1.78</v>
       </c>
       <c r="S16" s="32">
-        <v>2.17</v>
+        <v>1.97</v>
       </c>
       <c r="T16" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U16" s="31">
-        <v>1.82</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="V16" s="32">
         <v>2.08</v>
@@ -3009,22 +2983,22 @@
         <v>0</v>
       </c>
       <c r="P17" s="32">
-        <v>2.83</v>
+        <v>1.9</v>
       </c>
       <c r="Q17" s="32">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R17" s="32">
-        <v>1.5</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="S17" s="32">
-        <v>1.85</v>
+        <v>1.88</v>
       </c>
       <c r="T17" s="31">
         <v>2.5</v>
       </c>
       <c r="U17" s="31">
-        <v>2.13</v>
+        <v>2.1</v>
       </c>
       <c r="V17" s="32">
         <v>2.11</v>
@@ -3101,13 +3075,13 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="S18" s="32">
-        <v>2.65</v>
+        <v>1.89</v>
       </c>
       <c r="T18" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U18" s="31">
-        <v>1.57</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="V18" s="32">
         <v>3.03</v>
@@ -3141,7 +3115,7 @@
       <c r="D19" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="48">
         <v>7643</v>
       </c>
       <c r="F19" s="31">
@@ -3153,7 +3127,7 @@
       <c r="H19" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="48">
         <v>1043</v>
       </c>
       <c r="J19" s="31">
@@ -3175,22 +3149,22 @@
         <v>0</v>
       </c>
       <c r="P19" s="31">
-        <v>1.84</v>
+        <v>1.76</v>
       </c>
       <c r="Q19" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R19" s="32">
-        <v>2.11</v>
+        <v>2.17</v>
       </c>
       <c r="S19" s="32">
-        <v>2.4</v>
+        <v>2.09</v>
       </c>
       <c r="T19" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U19" s="31">
-        <v>1.66</v>
+        <v>1.93</v>
       </c>
       <c r="V19" s="31">
         <v>4.6399999999999997</v>
@@ -3224,7 +3198,7 @@
       <c r="D20" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="47">
+      <c r="E20" s="48">
         <v>36</v>
       </c>
       <c r="F20" s="31">
@@ -3236,7 +3210,7 @@
       <c r="H20" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="I20" s="47">
+      <c r="I20" s="48">
         <v>21</v>
       </c>
       <c r="J20" s="31">
@@ -3258,13 +3232,13 @@
         <v>0</v>
       </c>
       <c r="P20" s="31">
-        <v>2.92</v>
+        <v>1.92</v>
       </c>
       <c r="Q20" s="32">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R20" s="32">
-        <v>1.44</v>
+        <v>2.06</v>
       </c>
       <c r="S20" s="32">
         <v>1.9</v>
@@ -3307,7 +3281,7 @@
       <c r="D21" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="47">
+      <c r="E21" s="48">
         <v>16</v>
       </c>
       <c r="F21" s="31">
@@ -3319,7 +3293,7 @@
       <c r="H21" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="I21" s="47">
+      <c r="I21" s="48">
         <v>37</v>
       </c>
       <c r="J21" s="31">
@@ -3341,13 +3315,13 @@
         <v>0</v>
       </c>
       <c r="P21" s="31">
-        <v>1.45</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="Q21" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R21" s="32">
-        <v>2.85</v>
+        <v>1.87</v>
       </c>
       <c r="S21" s="32">
         <v>2.1</v>
@@ -3424,22 +3398,22 @@
         <v>0</v>
       </c>
       <c r="P22" s="31">
-        <v>1.59</v>
+        <v>1.92</v>
       </c>
       <c r="Q22" s="32">
         <v>0.5</v>
       </c>
       <c r="R22" s="32">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="S22" s="32">
-        <v>1.49</v>
+        <v>1.97</v>
       </c>
       <c r="T22" s="31">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="U22" s="31">
-        <v>2.82</v>
+        <v>1.96</v>
       </c>
       <c r="V22" s="31">
         <v>3.8</v>
@@ -3507,13 +3481,13 @@
         <v>0</v>
       </c>
       <c r="P23" s="31">
-        <v>1.47</v>
+        <v>2.09</v>
       </c>
       <c r="Q23" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R23" s="32">
-        <v>2.85</v>
+        <v>1.85</v>
       </c>
       <c r="S23" s="32">
         <v>2.09</v>
@@ -3599,13 +3573,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="S24" s="32">
-        <v>2.35</v>
+        <v>2.08</v>
       </c>
       <c r="T24" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U24" s="31">
-        <v>1.72</v>
+        <v>1.93</v>
       </c>
       <c r="V24" s="31">
         <v>2.79</v>
@@ -3673,13 +3647,13 @@
         <v>0</v>
       </c>
       <c r="P25" s="31">
-        <v>3.22</v>
+        <v>2.17</v>
       </c>
       <c r="Q25" s="32">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R25" s="32">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="S25" s="32">
         <v>1.94</v>
@@ -3756,19 +3730,19 @@
         <v>0</v>
       </c>
       <c r="P26" s="31">
-        <v>1.5</v>
-      </c>
-      <c r="Q26" s="32">
-        <v>0.5</v>
+        <v>1.85</v>
+      </c>
+      <c r="Q26" s="31">
+        <v>1</v>
       </c>
       <c r="R26" s="32">
-        <v>2.65</v>
+        <v>2.13</v>
       </c>
       <c r="S26" s="32">
         <v>2.0499999999999998</v>
       </c>
       <c r="T26" s="31">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="U26" s="31">
         <v>1.85</v>
@@ -3839,13 +3813,13 @@
         <v>0</v>
       </c>
       <c r="P27" s="31">
-        <v>2.85</v>
-      </c>
-      <c r="Q27" s="32">
-        <v>1.5</v>
+        <v>1.94</v>
+      </c>
+      <c r="Q27" s="31">
+        <v>1</v>
       </c>
       <c r="R27" s="32">
-        <v>1.45</v>
+        <v>2</v>
       </c>
       <c r="S27" s="32">
         <v>1.96</v>
@@ -3922,22 +3896,22 @@
         <v>0</v>
       </c>
       <c r="P28" s="31">
-        <v>1.47</v>
-      </c>
-      <c r="Q28" s="32">
-        <v>0.5</v>
+        <v>2.16</v>
+      </c>
+      <c r="Q28" s="31">
+        <v>1</v>
       </c>
       <c r="R28" s="32">
-        <v>2.83</v>
+        <v>1.83</v>
       </c>
       <c r="S28" s="32">
-        <v>2.12</v>
+        <v>1.84</v>
       </c>
       <c r="T28" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U28" s="31">
-        <v>1.84</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="V28" s="31">
         <v>2.54</v>
@@ -4005,13 +3979,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="31">
-        <v>1.43</v>
-      </c>
-      <c r="Q29" s="32">
-        <v>0.5</v>
+        <v>1.97</v>
+      </c>
+      <c r="Q29" s="31">
+        <v>1</v>
       </c>
       <c r="R29" s="32">
-        <v>2.95</v>
+        <v>1.95</v>
       </c>
       <c r="S29" s="32">
         <v>1.99</v>
@@ -4097,13 +4071,13 @@
         <v>2.08</v>
       </c>
       <c r="S30" s="32">
-        <v>1.48</v>
+        <v>1.87</v>
       </c>
       <c r="T30" s="31">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="U30" s="31">
-        <v>2.95</v>
+        <v>2.11</v>
       </c>
       <c r="V30" s="31">
         <v>5.55</v>
@@ -4171,22 +4145,22 @@
         <v>0</v>
       </c>
       <c r="P31" s="31">
-        <v>1.61</v>
+        <v>1.92</v>
       </c>
       <c r="Q31" s="31">
         <v>0.5</v>
       </c>
       <c r="R31" s="31">
-        <v>2.4700000000000002</v>
+        <v>2</v>
       </c>
       <c r="S31" s="32">
-        <v>1.54</v>
+        <v>1.97</v>
       </c>
       <c r="T31" s="31">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="U31" s="31">
-        <v>2.69</v>
+        <v>1.96</v>
       </c>
       <c r="V31" s="31">
         <v>3.52</v>
@@ -4254,13 +4228,13 @@
         <v>0</v>
       </c>
       <c r="P32" s="31">
-        <v>3.04</v>
-      </c>
-      <c r="Q32" s="32">
-        <v>1.5</v>
+        <v>1.97</v>
+      </c>
+      <c r="Q32" s="31">
+        <v>1</v>
       </c>
       <c r="R32" s="31">
-        <v>1.45</v>
+        <v>1.94</v>
       </c>
       <c r="S32" s="32">
         <v>1.96</v>
@@ -4337,22 +4311,22 @@
         <v>0</v>
       </c>
       <c r="P33" s="31">
-        <v>1.51</v>
+        <v>1.72</v>
       </c>
       <c r="Q33" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R33" s="31">
-        <v>2.7</v>
+        <v>2.23</v>
       </c>
       <c r="S33" s="32">
-        <v>2.25</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="T33" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U33" s="31">
-        <v>1.75</v>
+        <v>1.98</v>
       </c>
       <c r="V33" s="31">
         <v>2.85</v>
@@ -4420,13 +4394,13 @@
         <v>0</v>
       </c>
       <c r="P34" s="31">
-        <v>1.53</v>
+        <v>1.71</v>
       </c>
       <c r="Q34" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R34" s="31">
-        <v>2.63</v>
+        <v>2.16</v>
       </c>
       <c r="S34" s="32">
         <v>1.96</v>
@@ -4512,13 +4486,13 @@
         <v>1.7</v>
       </c>
       <c r="S35" s="32">
-        <v>2.75</v>
+        <v>1.85</v>
       </c>
       <c r="T35" s="31">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U35" s="31">
-        <v>1.56</v>
+        <v>2.06</v>
       </c>
       <c r="V35" s="31">
         <v>1.83</v>
@@ -4586,13 +4560,13 @@
         <v>0</v>
       </c>
       <c r="P36" s="31">
-        <v>1.49</v>
+        <v>1.95</v>
       </c>
       <c r="Q36" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R36" s="31">
-        <v>2.7</v>
+        <v>1.95</v>
       </c>
       <c r="S36" s="32">
         <v>1.99</v>
@@ -4678,13 +4652,13 @@
         <v>3</v>
       </c>
       <c r="S37" s="32">
-        <v>2.16</v>
+        <v>1.51</v>
       </c>
       <c r="T37" s="31">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="U37" s="31">
-        <v>1.9</v>
+        <v>2.75</v>
       </c>
       <c r="V37" s="31">
         <v>6.35</v>
@@ -4835,22 +4809,22 @@
         <v>0</v>
       </c>
       <c r="P39" s="31">
-        <v>2.85</v>
+        <v>1.87</v>
       </c>
       <c r="Q39" s="31">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R39" s="31">
-        <v>1.45</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="S39" s="32">
-        <v>1.97</v>
+        <v>1.95</v>
       </c>
       <c r="T39" s="31">
         <v>2.5</v>
       </c>
       <c r="U39" s="31">
-        <v>1.98</v>
+        <v>1.95</v>
       </c>
       <c r="V39" s="31">
         <v>13</v>
@@ -5001,13 +4975,13 @@
         <v>0</v>
       </c>
       <c r="P41" s="31">
-        <v>1.45</v>
+        <v>1.93</v>
       </c>
       <c r="Q41" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R41" s="31">
-        <v>2.97</v>
+        <v>1.97</v>
       </c>
       <c r="S41" s="32">
         <v>2.0499999999999998</v>
@@ -5084,10 +5058,10 @@
         <v>0</v>
       </c>
       <c r="P42" s="31">
-        <v>1.52</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="Q42" s="31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R42" s="31">
         <v>1.74</v>
@@ -5252,8 +5226,8 @@
       <c r="P44" s="31">
         <v>1.67</v>
       </c>
-      <c r="Q44" s="32">
-        <v>0.5</v>
+      <c r="Q44" s="31">
+        <v>1</v>
       </c>
       <c r="R44" s="31">
         <v>2.25</v>
@@ -5333,22 +5307,22 @@
         <v>0</v>
       </c>
       <c r="P45" s="31">
-        <v>2.67</v>
+        <v>1.31</v>
       </c>
       <c r="Q45" s="31">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="R45" s="31">
-        <v>1.53</v>
+        <v>3.5</v>
       </c>
       <c r="S45" s="32">
-        <v>2.98</v>
+        <v>2.06</v>
       </c>
       <c r="T45" s="31">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U45" s="31">
-        <v>1.5</v>
+        <v>1.85</v>
       </c>
       <c r="V45" s="31">
         <v>8.5</v>
@@ -5416,13 +5390,13 @@
         <v>0</v>
       </c>
       <c r="P46" s="31">
-        <v>1.49</v>
-      </c>
-      <c r="Q46" s="32">
-        <v>0.5</v>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="Q46" s="31">
+        <v>1</v>
       </c>
       <c r="R46" s="31">
-        <v>2.7</v>
+        <v>1.85</v>
       </c>
       <c r="S46" s="32">
         <v>2.17</v>
@@ -5499,13 +5473,13 @@
         <v>0</v>
       </c>
       <c r="P47" s="31">
-        <v>2.88</v>
+        <v>1.88</v>
       </c>
       <c r="Q47" s="31">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="R47" s="31">
-        <v>1.45</v>
+        <v>2.02</v>
       </c>
       <c r="S47" s="32">
         <v>1.98</v>
@@ -5591,13 +5565,13 @@
         <v>1.53</v>
       </c>
       <c r="S48" s="32">
+        <v>2.23</v>
+      </c>
+      <c r="T48" s="31">
+        <v>3</v>
+      </c>
+      <c r="U48" s="31">
         <v>1.78</v>
-      </c>
-      <c r="T48" s="31">
-        <v>2.5</v>
-      </c>
-      <c r="U48" s="31">
-        <v>2.3199999999999998</v>
       </c>
       <c r="V48" s="31">
         <v>8.9</v>
@@ -5665,13 +5639,13 @@
         <v>0</v>
       </c>
       <c r="P49" s="31">
-        <v>1.48</v>
-      </c>
-      <c r="Q49" s="32">
-        <v>0.5</v>
+        <v>1.97</v>
+      </c>
+      <c r="Q49" s="31">
+        <v>1</v>
       </c>
       <c r="R49" s="31">
-        <v>2.75</v>
+        <v>1.93</v>
       </c>
       <c r="S49" s="32">
         <v>2.04</v>
@@ -5730,7 +5704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF9900"/>
@@ -5806,65 +5780,65 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="43" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="33" t="s">
+      <c r="F6" s="46"/>
+      <c r="G6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="39" t="s">
+      <c r="I6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="46" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="33" t="s">
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="39" t="s">
+      <c r="K7" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="40"/>
-      <c r="M7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="42"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
       <c r="K8" s="7">
         <v>20</v>
       </c>
@@ -5896,7 +5870,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="37" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -5930,7 +5904,7 @@
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
-      <c r="D11" s="37"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
@@ -5954,7 +5928,7 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
-      <c r="D12" s="37"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="3" t="s">
         <v>13</v>
       </c>
@@ -5980,7 +5954,7 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
-      <c r="D13" s="37"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="3" t="s">
         <v>24</v>
       </c>
@@ -6008,7 +5982,7 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
-      <c r="D14" s="37"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="9" t="s">
         <v>1</v>
       </c>
@@ -6035,7 +6009,7 @@
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
-      <c r="D15" s="37"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="9" t="s">
         <v>1</v>
       </c>
@@ -6062,7 +6036,7 @@
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
-      <c r="D16" s="37"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="9" t="s">
         <v>1</v>
       </c>
@@ -6089,7 +6063,7 @@
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
-      <c r="D17" s="37"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="9" t="s">
         <v>1</v>
       </c>
@@ -6122,7 +6096,7 @@
         <v>31</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="39" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="13" t="s">
@@ -6147,7 +6121,7 @@
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="37"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="13" t="s">
         <v>13</v>
       </c>
@@ -6170,7 +6144,7 @@
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
-      <c r="D20" s="37"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="13" t="s">
         <v>13</v>
       </c>
@@ -6193,7 +6167,7 @@
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="37"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="20" t="s">
         <v>1</v>
       </c>

</xml_diff>